<commit_message>
poprawki do wersji dla Banku
</commit_message>
<xml_diff>
--- a/dokumentacja/opisyFunkcji.xlsx
+++ b/dokumentacja/opisyFunkcji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>funkcjonalność / test</t>
   </si>
@@ -130,6 +130,54 @@
   </si>
   <si>
     <t>test.kartyUsuniecieAutomatycznejSplatyCalkowitej.js</t>
+  </si>
+  <si>
+    <t>przelew do US</t>
+  </si>
+  <si>
+    <t>dodanie odbiorcy krajowego</t>
+  </si>
+  <si>
+    <t>dodanie i edycja odbiorcy krajowego</t>
+  </si>
+  <si>
+    <t>dodnie i usuniecie odbiorcy krajowego</t>
+  </si>
+  <si>
+    <t>aktywacja karty</t>
+  </si>
+  <si>
+    <t>dodanie automatycznej splaty całkowitej</t>
+  </si>
+  <si>
+    <t>dodanie automatycznej splaty minimalnej</t>
+  </si>
+  <si>
+    <t>spłata karty</t>
+  </si>
+  <si>
+    <t>usunięcie automatycznej splaty minimalnej</t>
+  </si>
+  <si>
+    <t>usunięcie automatycznej splaty całkowitej</t>
+  </si>
+  <si>
+    <t>zasrzeżenie karty</t>
+  </si>
+  <si>
+    <t>zmiana limitu karty</t>
+  </si>
+  <si>
+    <t>zmiana pin karty</t>
+  </si>
+  <si>
+    <t>test.przelewWlasny.js</t>
+  </si>
+  <si>
+    <t>rachunekOdbiorcy,tytulPrzelewu,kwota,hasloSms</t>
+  </si>
+  <si>
+    <t>przelew własny</t>
   </si>
 </sst>
 </file>
@@ -503,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -571,6 +619,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -582,19 +633,25 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -604,94 +661,138 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
       <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>